<commit_message>
Create new tabel in database and update in energy-analysis
</commit_message>
<xml_diff>
--- a/src/ExcelImport/importfile.xlsx
+++ b/src/ExcelImport/importfile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\takl23\dbwebb-kurser\mvc\me\report\src\ExcelImport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{861106C0-A540-471F-976E-B5A0098F1674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A85CE9-67F3-4ADD-849C-F8D4D8BB93BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elområde och län" sheetId="9" r:id="rId1"/>
@@ -114,9 +114,6 @@
     <t>https://www.scb.se/hitta-statistik/statistik-efter-amne/hushallens-ekonomi/inkomster-och-inkomstfordelning/</t>
   </si>
   <si>
-    <t>https://www.ei.se/sv/statistik/</t>
-  </si>
-  <si>
     <t>https://www.smhi.se/data/meteorologi/temperatur/</t>
   </si>
   <si>
@@ -298,6 +295,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>https://www.energimarknadsinspektionen.se/sv/statistik/elmarknad/elpriser/</t>
   </si>
 </sst>
 </file>
@@ -707,8 +707,8 @@
   </sheetPr>
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -718,15 +718,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>4</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>5</v>
@@ -742,7 +742,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>5</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>5</v>
@@ -758,7 +758,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>6</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>6</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>6</v>
@@ -782,7 +782,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>6</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>6</v>
@@ -798,7 +798,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>6</v>
@@ -806,7 +806,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>6</v>
@@ -814,7 +814,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>6</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>6</v>
@@ -830,7 +830,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>6</v>
@@ -838,7 +838,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>6</v>
@@ -846,7 +846,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>6</v>
@@ -854,7 +854,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>6</v>
@@ -862,7 +862,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>7</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>7</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>7</v>
@@ -886,7 +886,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>7</v>
@@ -921,64 +921,64 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>49</v>
-      </c>
       <c r="Q1" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.55000000000000004">
@@ -1602,7 +1602,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -1971,7 +1973,9 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -2157,7 +2161,9 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
@@ -2341,7 +2347,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection sqref="A1:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2542,64 +2548,64 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.55000000000000004">
@@ -3223,13 +3229,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="3" width="28.68359375" customWidth="1"/>
+    <col min="1" max="1" width="26.26171875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.41796875" customWidth="1"/>
     <col min="4" max="4" width="9.83984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="127.83984375" bestFit="1" customWidth="1"/>
   </cols>
@@ -3251,27 +3258,27 @@
         <v>12</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="E2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>88</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3285,13 +3292,13 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
         <v>31</v>
       </c>
-      <c r="E3" t="s">
-        <v>32</v>
-      </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3305,13 +3312,13 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3325,13 +3332,13 @@
         <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3341,17 +3348,17 @@
       <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>28</v>
+      <c r="C6" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3362,16 +3369,16 @@
         <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3382,36 +3389,36 @@
         <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
-        <v>31</v>
-      </c>
       <c r="E9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" t="s">
         <v>57</v>
-      </c>
-      <c r="F9" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ResetAndImportDataCommand for updating database, Update database
</commit_message>
<xml_diff>
--- a/src/ExcelImport/importfile.xlsx
+++ b/src/ExcelImport/importfile.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\takl23\dbwebb-kurser\mvc\me\report\src\ExcelImport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D573285-C911-4350-B16B-F01BD134FEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCCF8C2-89CD-4A11-8134-1F053E497853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elområde och län" sheetId="9" r:id="rId1"/>
     <sheet name="Befolkning per län" sheetId="1" r:id="rId2"/>
     <sheet name="Elpris per elområde och år" sheetId="4" r:id="rId3"/>
     <sheet name="Snittförbrukning per elområde" sheetId="6" r:id="rId4"/>
-    <sheet name="Referenser" sheetId="7" r:id="rId5"/>
+    <sheet name="7.3.1" sheetId="11" r:id="rId5"/>
+    <sheet name="7.2.1.1" sheetId="12" r:id="rId6"/>
+    <sheet name="7.2.1.2" sheetId="13" r:id="rId7"/>
+    <sheet name="Referenser" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="88">
   <si>
     <t>År</t>
   </si>
@@ -256,6 +259,51 @@
   </si>
   <si>
     <t>Gwh/år</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>VIM</t>
+  </si>
+  <si>
+    <t>El</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Biofuels (TWh)</t>
+  </si>
+  <si>
+    <t>Hydropower (TWh)</t>
+  </si>
+  <si>
+    <t>Wind Power (TWh)</t>
+  </si>
+  <si>
+    <t>Heat Pumps (TWh)</t>
+  </si>
+  <si>
+    <t>Solar Energy (TWh)</t>
+  </si>
+  <si>
+    <t>Total (TWh)</t>
+  </si>
+  <si>
+    <t>Stat Transfer to Norway (TWh)</t>
+  </si>
+  <si>
+    <t>Renewable Energy in Target Calculation (TWh)</t>
+  </si>
+  <si>
+    <t>Total Energy Use (TWh)</t>
   </si>
 </sst>
 </file>
@@ -353,8 +401,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1297,20 +1347,15 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:Y35"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A7" sqref="A7:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <cols>
-    <col min="14" max="14" width="23.83984375" customWidth="1"/>
-    <col min="15" max="16" width="9.83984375" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="7.68359375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1327,7 +1372,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -1344,7 +1389,7 @@
         <v>0.42087999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -1361,7 +1406,7 @@
         <v>0.26956999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -1378,7 +1423,7 @@
         <v>0.81865999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -1395,7 +1440,7 @@
         <v>1.6204799999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>2023</v>
       </c>
@@ -1411,84 +1456,6 @@
       <c r="E6" s="7">
         <v>0.74159000000000008</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="7"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="7"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
-      <c r="Y14" s="7"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="7"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="7"/>
-    </row>
-    <row r="20" spans="15:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-    </row>
-    <row r="31" spans="15:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
-    </row>
-    <row r="32" spans="15:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="P32" s="7"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="7"/>
-    </row>
-    <row r="33" spans="16:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="P33" s="7"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="7"/>
-    </row>
-    <row r="34" spans="16:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="P34" s="7"/>
-      <c r="Q34" s="7"/>
-      <c r="R34" s="7"/>
-      <c r="S34" s="7"/>
-    </row>
-    <row r="35" spans="16:19" x14ac:dyDescent="0.55000000000000004">
-      <c r="P35" s="7"/>
-      <c r="Q35" s="7"/>
-      <c r="R35" s="7"/>
-      <c r="S35" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1644,6 +1611,1070 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446A2D8C-1FAB-4D56-849C-7774E6B82ADB}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7">
+        <v>2021</v>
+      </c>
+      <c r="B2" s="7">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B3" s="7">
+        <v>-24.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B4" s="7">
+        <v>-21.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="7">
+        <v>2018</v>
+      </c>
+      <c r="B5" s="7">
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="7">
+        <v>2017</v>
+      </c>
+      <c r="B6" s="7">
+        <v>-16.899999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="7">
+        <v>2016</v>
+      </c>
+      <c r="B7" s="7">
+        <v>-14.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="7">
+        <v>2015</v>
+      </c>
+      <c r="B8" s="7">
+        <v>-18.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="7">
+        <v>2014</v>
+      </c>
+      <c r="B9" s="7">
+        <v>-10.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="7">
+        <v>2013</v>
+      </c>
+      <c r="B10" s="7">
+        <v>-5.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="7">
+        <v>2012</v>
+      </c>
+      <c r="B11" s="7">
+        <v>-1.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="7">
+        <v>2011</v>
+      </c>
+      <c r="B12" s="7">
+        <v>-4.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="7">
+        <v>2010</v>
+      </c>
+      <c r="B13" s="7">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="7">
+        <v>2009</v>
+      </c>
+      <c r="B14" s="7">
+        <v>-2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="7">
+        <v>2008</v>
+      </c>
+      <c r="B15" s="7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48644E9-3FCE-409F-8A79-26C12A3E78B0}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>2005</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>51</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>2006</v>
+      </c>
+      <c r="B3">
+        <v>53</v>
+      </c>
+      <c r="C3">
+        <v>52</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>2007</v>
+      </c>
+      <c r="B4">
+        <v>55</v>
+      </c>
+      <c r="C4">
+        <v>53</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>2008</v>
+      </c>
+      <c r="B5">
+        <v>57</v>
+      </c>
+      <c r="C5">
+        <v>54</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>2009</v>
+      </c>
+      <c r="B6">
+        <v>61</v>
+      </c>
+      <c r="C6">
+        <v>58</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>2010</v>
+      </c>
+      <c r="B7">
+        <v>58</v>
+      </c>
+      <c r="C7">
+        <v>56</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>2011</v>
+      </c>
+      <c r="B8">
+        <v>60</v>
+      </c>
+      <c r="C8">
+        <v>60</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>2012</v>
+      </c>
+      <c r="B9">
+        <v>62</v>
+      </c>
+      <c r="C9">
+        <v>60</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>2013</v>
+      </c>
+      <c r="B10">
+        <v>64</v>
+      </c>
+      <c r="C10">
+        <v>62</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>2014</v>
+      </c>
+      <c r="B11">
+        <v>64</v>
+      </c>
+      <c r="C11">
+        <v>63</v>
+      </c>
+      <c r="D11">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>2015</v>
+      </c>
+      <c r="B12">
+        <v>65</v>
+      </c>
+      <c r="C12">
+        <v>66</v>
+      </c>
+      <c r="D12">
+        <v>21</v>
+      </c>
+      <c r="E12">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>2016</v>
+      </c>
+      <c r="B13">
+        <v>65</v>
+      </c>
+      <c r="C13">
+        <v>65</v>
+      </c>
+      <c r="D13">
+        <v>27</v>
+      </c>
+      <c r="E13">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>2017</v>
+      </c>
+      <c r="B14">
+        <v>66</v>
+      </c>
+      <c r="C14">
+        <v>66</v>
+      </c>
+      <c r="D14">
+        <v>27</v>
+      </c>
+      <c r="E14">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>2018</v>
+      </c>
+      <c r="B15">
+        <v>65</v>
+      </c>
+      <c r="C15">
+        <v>66</v>
+      </c>
+      <c r="D15">
+        <v>30</v>
+      </c>
+      <c r="E15">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>2019</v>
+      </c>
+      <c r="B16">
+        <v>66</v>
+      </c>
+      <c r="C16">
+        <v>71</v>
+      </c>
+      <c r="D16">
+        <v>30</v>
+      </c>
+      <c r="E16">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>2020</v>
+      </c>
+      <c r="B17">
+        <v>66</v>
+      </c>
+      <c r="C17">
+        <v>74</v>
+      </c>
+      <c r="D17">
+        <v>32</v>
+      </c>
+      <c r="E17">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>2021</v>
+      </c>
+      <c r="B18">
+        <v>69</v>
+      </c>
+      <c r="C18">
+        <v>76</v>
+      </c>
+      <c r="D18">
+        <v>30</v>
+      </c>
+      <c r="E18">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>2022</v>
+      </c>
+      <c r="B19">
+        <v>69</v>
+      </c>
+      <c r="C19">
+        <v>83</v>
+      </c>
+      <c r="D19">
+        <v>29</v>
+      </c>
+      <c r="E19">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320DC7E3-85C4-4A17-9164-F72DD74E817C}">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="7">
+        <v>2021</v>
+      </c>
+      <c r="B2" s="7">
+        <v>134</v>
+      </c>
+      <c r="C2" s="7">
+        <v>67</v>
+      </c>
+      <c r="D2" s="7">
+        <v>29</v>
+      </c>
+      <c r="E2" s="7">
+        <v>19</v>
+      </c>
+      <c r="F2" s="7">
+        <v>2</v>
+      </c>
+      <c r="G2" s="7">
+        <v>250</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0</v>
+      </c>
+      <c r="I2" s="7">
+        <v>250</v>
+      </c>
+      <c r="J2" s="7">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="7">
+        <v>2020</v>
+      </c>
+      <c r="B3" s="7">
+        <v>131</v>
+      </c>
+      <c r="C3" s="7">
+        <v>67</v>
+      </c>
+      <c r="D3" s="7">
+        <v>25</v>
+      </c>
+      <c r="E3" s="7">
+        <v>18</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7">
+        <v>241</v>
+      </c>
+      <c r="H3" s="7">
+        <v>3</v>
+      </c>
+      <c r="I3" s="7">
+        <v>238</v>
+      </c>
+      <c r="J3" s="7">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B4" s="7">
+        <v>126</v>
+      </c>
+      <c r="C4" s="7">
+        <v>67</v>
+      </c>
+      <c r="D4" s="7">
+        <v>21</v>
+      </c>
+      <c r="E4" s="7">
+        <v>18</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7">
+        <v>232</v>
+      </c>
+      <c r="H4" s="7">
+        <v>6</v>
+      </c>
+      <c r="I4" s="7">
+        <v>226</v>
+      </c>
+      <c r="J4" s="7">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="7">
+        <v>2018</v>
+      </c>
+      <c r="B5" s="7">
+        <v>124</v>
+      </c>
+      <c r="C5" s="7">
+        <v>66</v>
+      </c>
+      <c r="D5" s="7">
+        <v>18</v>
+      </c>
+      <c r="E5" s="7">
+        <v>17</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7">
+        <v>226</v>
+      </c>
+      <c r="H5" s="7">
+        <v>5</v>
+      </c>
+      <c r="I5" s="7">
+        <v>221</v>
+      </c>
+      <c r="J5" s="7">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="7">
+        <v>2017</v>
+      </c>
+      <c r="B6" s="7">
+        <v>126</v>
+      </c>
+      <c r="C6" s="7">
+        <v>66</v>
+      </c>
+      <c r="D6" s="7">
+        <v>17</v>
+      </c>
+      <c r="E6" s="7">
+        <v>16</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7">
+        <v>226</v>
+      </c>
+      <c r="H6" s="7">
+        <v>5</v>
+      </c>
+      <c r="I6" s="7">
+        <v>220</v>
+      </c>
+      <c r="J6" s="7">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="7">
+        <v>2016</v>
+      </c>
+      <c r="B7" s="7">
+        <v>123</v>
+      </c>
+      <c r="C7" s="7">
+        <v>66</v>
+      </c>
+      <c r="D7" s="7">
+        <v>16</v>
+      </c>
+      <c r="E7" s="7">
+        <v>16</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7">
+        <v>221</v>
+      </c>
+      <c r="H7" s="7">
+        <v>5</v>
+      </c>
+      <c r="I7" s="7">
+        <v>216</v>
+      </c>
+      <c r="J7" s="7">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="7">
+        <v>2015</v>
+      </c>
+      <c r="B8" s="7">
+        <v>118</v>
+      </c>
+      <c r="C8" s="7">
+        <v>67</v>
+      </c>
+      <c r="D8" s="7">
+        <v>14</v>
+      </c>
+      <c r="E8" s="7">
+        <v>14</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7">
+        <v>213</v>
+      </c>
+      <c r="H8" s="7">
+        <v>4</v>
+      </c>
+      <c r="I8" s="7">
+        <v>209</v>
+      </c>
+      <c r="J8" s="7">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="7">
+        <v>2014</v>
+      </c>
+      <c r="B9" s="7">
+        <v>113</v>
+      </c>
+      <c r="C9" s="7">
+        <v>65</v>
+      </c>
+      <c r="D9" s="7">
+        <v>11</v>
+      </c>
+      <c r="E9" s="7">
+        <v>14</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
+      <c r="G9" s="7">
+        <v>204</v>
+      </c>
+      <c r="H9" s="7">
+        <v>3</v>
+      </c>
+      <c r="I9" s="7">
+        <v>201</v>
+      </c>
+      <c r="J9" s="7">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="7">
+        <v>2013</v>
+      </c>
+      <c r="B10" s="7">
+        <v>114</v>
+      </c>
+      <c r="C10" s="7">
+        <v>68</v>
+      </c>
+      <c r="D10" s="7">
+        <v>9</v>
+      </c>
+      <c r="E10" s="7">
+        <v>14</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7">
+        <v>205</v>
+      </c>
+      <c r="H10" s="7">
+        <v>2</v>
+      </c>
+      <c r="I10" s="7">
+        <v>203</v>
+      </c>
+      <c r="J10" s="7">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="7">
+        <v>2012</v>
+      </c>
+      <c r="B11" s="7">
+        <v>115</v>
+      </c>
+      <c r="C11" s="7">
+        <v>69</v>
+      </c>
+      <c r="D11" s="7">
+        <v>7</v>
+      </c>
+      <c r="E11" s="7">
+        <v>14</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7">
+        <v>205</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7">
+        <v>205</v>
+      </c>
+      <c r="J11" s="7">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="7">
+        <v>2011</v>
+      </c>
+      <c r="B12" s="7">
+        <v>108</v>
+      </c>
+      <c r="C12" s="7">
+        <v>69</v>
+      </c>
+      <c r="D12" s="7">
+        <v>5</v>
+      </c>
+      <c r="E12" s="7">
+        <v>14</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7">
+        <v>196</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7">
+        <v>196</v>
+      </c>
+      <c r="J12" s="7">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="7">
+        <v>2010</v>
+      </c>
+      <c r="B13" s="7">
+        <v>114</v>
+      </c>
+      <c r="C13" s="7">
+        <v>68</v>
+      </c>
+      <c r="D13" s="7">
+        <v>3</v>
+      </c>
+      <c r="E13" s="7">
+        <v>11</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7">
+        <v>197</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7">
+        <v>197</v>
+      </c>
+      <c r="J13" s="7">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="7">
+        <v>2009</v>
+      </c>
+      <c r="B14" s="7">
+        <v>104</v>
+      </c>
+      <c r="C14" s="7">
+        <v>68</v>
+      </c>
+      <c r="D14" s="7">
+        <v>3</v>
+      </c>
+      <c r="E14" s="7">
+        <v>11</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7">
+        <v>186</v>
+      </c>
+      <c r="H14" s="7">
+        <v>0</v>
+      </c>
+      <c r="I14" s="7">
+        <v>186</v>
+      </c>
+      <c r="J14" s="7">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="7">
+        <v>2008</v>
+      </c>
+      <c r="B15" s="7">
+        <v>101</v>
+      </c>
+      <c r="C15" s="7">
+        <v>67</v>
+      </c>
+      <c r="D15" s="7">
+        <v>2</v>
+      </c>
+      <c r="E15" s="7">
+        <v>10</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0</v>
+      </c>
+      <c r="G15" s="7">
+        <v>180</v>
+      </c>
+      <c r="H15" s="7">
+        <v>0</v>
+      </c>
+      <c r="I15" s="7">
+        <v>180</v>
+      </c>
+      <c r="J15" s="7">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="7">
+        <v>2007</v>
+      </c>
+      <c r="B16" s="7">
+        <v>100</v>
+      </c>
+      <c r="C16" s="7">
+        <v>69</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
+      <c r="E16" s="7">
+        <v>9</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0</v>
+      </c>
+      <c r="G16" s="7">
+        <v>179</v>
+      </c>
+      <c r="H16" s="7">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7">
+        <v>179</v>
+      </c>
+      <c r="J16" s="7">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="7">
+        <v>2006</v>
+      </c>
+      <c r="B17" s="7">
+        <v>95</v>
+      </c>
+      <c r="C17" s="7">
+        <v>68</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7">
+        <v>8</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7">
+        <v>172</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0</v>
+      </c>
+      <c r="I17" s="7">
+        <v>172</v>
+      </c>
+      <c r="J17" s="7">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="7">
+        <v>2005</v>
+      </c>
+      <c r="B18" s="7">
+        <v>89</v>
+      </c>
+      <c r="C18" s="7">
+        <v>68</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1</v>
+      </c>
+      <c r="E18" s="7">
+        <v>7</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0</v>
+      </c>
+      <c r="G18" s="7">
+        <v>165</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0</v>
+      </c>
+      <c r="I18" s="7">
+        <v>165</v>
+      </c>
+      <c r="J18" s="7">
+        <v>413</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
@@ -1687,7 +2718,7 @@
       <c r="B2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>70</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -1707,7 +2738,7 @@
       <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>69</v>
       </c>
       <c r="D3" t="s">
@@ -1724,7 +2755,7 @@
       <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>68</v>
       </c>
       <c r="D4" t="s">
@@ -1741,7 +2772,7 @@
       <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>71</v>
       </c>
       <c r="D5" t="s">

</xml_diff>